<commit_message>
Add remove_empty_cols function Update lab_info.xlsx
</commit_message>
<xml_diff>
--- a/lab_info.xlsx
+++ b/lab_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bigdata\my_packages\labbinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E152B49D-8613-41C6-8F4C-2D3932087376}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31845ED9-70B2-47DF-B234-D6D1F45C4A93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,7 +924,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1081,6 +1081,15 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -1510,8 +1519,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1872,30 +1884,30 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,7 +1915,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1912,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1937,7 +1949,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1946,7 +1958,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1954,7 +1966,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1963,7 +1975,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1971,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1980,7 +1992,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2107,7 +2119,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -2116,7 +2128,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,7 +2136,7 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -2133,7 +2145,7 @@
         <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2153,16 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,7 +2187,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -2184,7 +2196,7 @@
         <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,10 +2204,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
         <v>32</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2203,7 +2215,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -2212,7 +2224,7 @@
         <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2220,7 +2232,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
@@ -2229,7 +2241,7 @@
         <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2237,7 +2249,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -2246,7 +2258,7 @@
         <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2254,7 +2266,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
@@ -2263,7 +2275,7 @@
         <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2271,7 +2283,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>42</v>
@@ -2280,7 +2292,7 @@
         <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2305,7 +2317,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -2314,7 +2326,7 @@
         <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2322,7 +2334,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
@@ -2331,7 +2343,7 @@
         <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2339,7 +2351,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>49</v>
@@ -2348,7 +2360,7 @@
         <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2356,7 +2368,7 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -2365,7 +2377,7 @@
         <v>51</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2373,7 +2385,7 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
         <v>53</v>
@@ -2382,7 +2394,7 @@
         <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2390,7 +2402,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>55</v>
@@ -2399,7 +2411,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -2407,7 +2419,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
         <v>57</v>
@@ -2416,7 +2428,7 @@
         <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -2424,7 +2436,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
         <v>59</v>
@@ -2433,7 +2445,7 @@
         <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -2441,7 +2453,7 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
         <v>61</v>
@@ -2450,7 +2462,7 @@
         <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2458,7 +2470,7 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
         <v>63</v>
@@ -2467,7 +2479,7 @@
         <v>63</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -2475,7 +2487,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
         <v>65</v>
@@ -2484,7 +2496,7 @@
         <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -2492,10 +2504,10 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" t="s">
         <v>67</v>
-      </c>
-      <c r="E37" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2503,10 +2515,10 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" t="s">
         <v>69</v>
-      </c>
-      <c r="E38" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -2514,7 +2526,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
         <v>71</v>
@@ -2523,7 +2535,7 @@
         <v>71</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -2531,16 +2543,16 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
         <v>73</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>73</v>
-      </c>
-      <c r="D40" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -2551,10 +2563,10 @@
         <v>76</v>
       </c>
       <c r="C41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" t="s">
         <v>76</v>
-      </c>
-      <c r="D41" t="s">
-        <v>77</v>
       </c>
       <c r="E41" t="s">
         <v>76</v>
@@ -2582,7 +2594,7 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
         <v>79</v>
@@ -2591,7 +2603,7 @@
         <v>79</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2599,10 +2611,10 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" t="s">
         <v>81</v>
-      </c>
-      <c r="E44" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2612,7 +2624,7 @@
       <c r="B45" t="s">
         <v>83</v>
       </c>
-      <c r="D45" t="s">
+      <c r="C45" t="s">
         <v>83</v>
       </c>
       <c r="E45" t="s">
@@ -2626,7 +2638,7 @@
       <c r="B46" t="s">
         <v>84</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C46" t="s">
         <v>84</v>
       </c>
       <c r="E46" t="s">
@@ -2638,16 +2650,16 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
+        <v>298</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
         <v>85</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>85</v>
-      </c>
-      <c r="D47" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -2655,13 +2667,13 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
         <v>87</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>87</v>
-      </c>
-      <c r="E48" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2669,13 +2681,13 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" t="s">
         <v>89</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>89</v>
-      </c>
-      <c r="E49" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,7 +2695,7 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
         <v>91</v>
@@ -2692,7 +2704,7 @@
         <v>91</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,13 +2712,13 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" t="s">
         <v>93</v>
-      </c>
-      <c r="D51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E51" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2714,13 +2726,13 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
         <v>96</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>96</v>
-      </c>
-      <c r="E52" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2728,10 +2740,10 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" t="s">
         <v>98</v>
-      </c>
-      <c r="E53" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2739,10 +2751,10 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" t="s">
         <v>100</v>
-      </c>
-      <c r="E54" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2750,10 +2762,10 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" t="s">
         <v>102</v>
-      </c>
-      <c r="E55" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2761,10 +2773,10 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
         <v>104</v>
-      </c>
-      <c r="E56" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2772,10 +2784,10 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
+        <v>107</v>
+      </c>
+      <c r="E57" t="s">
         <v>106</v>
-      </c>
-      <c r="E57" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2783,10 +2795,10 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" t="s">
         <v>108</v>
-      </c>
-      <c r="E58" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2794,10 +2806,10 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" t="s">
         <v>110</v>
-      </c>
-      <c r="E59" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2805,10 +2817,10 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" t="s">
         <v>112</v>
-      </c>
-      <c r="E60" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2816,10 +2828,10 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
+        <v>115</v>
+      </c>
+      <c r="E61" t="s">
         <v>114</v>
-      </c>
-      <c r="E61" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2871,10 +2883,10 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
+        <v>115</v>
+      </c>
+      <c r="E66" t="s">
         <v>117</v>
-      </c>
-      <c r="E66" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2882,10 +2894,10 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
+        <v>116</v>
+      </c>
+      <c r="E67" t="s">
         <v>118</v>
-      </c>
-      <c r="E67" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2893,10 +2905,10 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E68" t="s">
         <v>119</v>
-      </c>
-      <c r="E68" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2904,10 +2916,10 @@
         <v>5</v>
       </c>
       <c r="B69" t="s">
+        <v>121</v>
+      </c>
+      <c r="E69" t="s">
         <v>120</v>
-      </c>
-      <c r="E69" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2927,16 @@
         <v>122</v>
       </c>
       <c r="B70" t="s">
+        <v>123</v>
+      </c>
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" t="s">
         <v>107</v>
       </c>
-      <c r="C70" t="s">
+      <c r="E70" t="s">
         <v>107</v>
-      </c>
-      <c r="D70" t="s">
-        <v>106</v>
-      </c>
-      <c r="E70" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2934,7 +2946,7 @@
       <c r="B71" t="s">
         <v>124</v>
       </c>
-      <c r="D71" t="s">
+      <c r="C71" t="s">
         <v>125</v>
       </c>
       <c r="E71" t="s">
@@ -2946,16 +2958,16 @@
         <v>122</v>
       </c>
       <c r="B72" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" t="s">
         <v>126</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>126</v>
-      </c>
-      <c r="D72" t="s">
-        <v>127</v>
-      </c>
-      <c r="E72" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2963,7 +2975,7 @@
         <v>122</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C73" t="s">
         <v>129</v>
@@ -2972,7 +2984,7 @@
         <v>129</v>
       </c>
       <c r="E73" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2980,7 +2992,7 @@
         <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C74" t="s">
         <v>131</v>
@@ -2989,7 +3001,7 @@
         <v>131</v>
       </c>
       <c r="E74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2997,7 +3009,7 @@
         <v>122</v>
       </c>
       <c r="B75" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="C75" t="s">
         <v>26</v>
@@ -3006,18 +3018,18 @@
         <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>122</v>
       </c>
-      <c r="D76" t="s">
+      <c r="B76" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" t="s">
         <v>134</v>
-      </c>
-      <c r="E76" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -3025,7 +3037,7 @@
         <v>122</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C77" t="s">
         <v>136</v>
@@ -3034,7 +3046,7 @@
         <v>136</v>
       </c>
       <c r="E77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -3042,7 +3054,7 @@
         <v>122</v>
       </c>
       <c r="B78" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C78" t="s">
         <v>138</v>
@@ -3051,7 +3063,7 @@
         <v>138</v>
       </c>
       <c r="E78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -3059,16 +3071,16 @@
         <v>122</v>
       </c>
       <c r="B79" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" t="s">
         <v>140</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
         <v>140</v>
-      </c>
-      <c r="D79" t="s">
-        <v>141</v>
-      </c>
-      <c r="E79" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -3076,16 +3088,16 @@
         <v>122</v>
       </c>
       <c r="B80" t="s">
+        <v>145</v>
+      </c>
+      <c r="C80" t="s">
+        <v>144</v>
+      </c>
+      <c r="D80" t="s">
+        <v>143</v>
+      </c>
+      <c r="E80" t="s">
         <v>10</v>
-      </c>
-      <c r="C80" t="s">
-        <v>143</v>
-      </c>
-      <c r="D80" t="s">
-        <v>144</v>
-      </c>
-      <c r="E80" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -3093,38 +3105,38 @@
         <v>122</v>
       </c>
       <c r="B81" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" t="s">
+        <v>146</v>
+      </c>
+      <c r="E81" t="s">
         <v>12</v>
-      </c>
-      <c r="C81" t="s">
-        <v>146</v>
-      </c>
-      <c r="D81" t="s">
-        <v>147</v>
-      </c>
-      <c r="E81" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>122</v>
       </c>
-      <c r="C82" t="s">
+      <c r="B82" t="s">
+        <v>150</v>
+      </c>
+      <c r="D82" t="s">
         <v>149</v>
-      </c>
-      <c r="E82" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>122</v>
       </c>
-      <c r="C83" t="s">
+      <c r="B83" t="s">
+        <v>152</v>
+      </c>
+      <c r="D83" t="s">
         <v>151</v>
-      </c>
-      <c r="E83" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -3132,123 +3144,123 @@
         <v>122</v>
       </c>
       <c r="B84" t="s">
+        <v>154</v>
+      </c>
+      <c r="D84" t="s">
         <v>153</v>
       </c>
-      <c r="C84" t="s">
+      <c r="E84" t="s">
         <v>153</v>
-      </c>
-      <c r="E84" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>122</v>
       </c>
-      <c r="D85" t="s">
+      <c r="B85" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" t="s">
         <v>155</v>
-      </c>
-      <c r="E85" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>122</v>
       </c>
-      <c r="D86" t="s">
+      <c r="B86" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" t="s">
         <v>156</v>
-      </c>
-      <c r="E86" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>122</v>
       </c>
-      <c r="D87" t="s">
+      <c r="B87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C87" t="s">
         <v>157</v>
-      </c>
-      <c r="E87" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>122</v>
       </c>
-      <c r="D88" t="s">
+      <c r="B88" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" t="s">
         <v>158</v>
-      </c>
-      <c r="E88" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>122</v>
       </c>
-      <c r="D89" t="s">
+      <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" t="s">
         <v>159</v>
-      </c>
-      <c r="E89" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>122</v>
       </c>
-      <c r="D90" t="s">
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90" t="s">
         <v>160</v>
-      </c>
-      <c r="E90" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>122</v>
       </c>
-      <c r="D91" t="s">
+      <c r="B91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" t="s">
         <v>161</v>
-      </c>
-      <c r="E91" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>122</v>
       </c>
-      <c r="D92" t="s">
+      <c r="B92" t="s">
+        <v>137</v>
+      </c>
+      <c r="C92" t="s">
         <v>162</v>
-      </c>
-      <c r="E92" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>122</v>
       </c>
-      <c r="D93" t="s">
+      <c r="B93" t="s">
+        <v>139</v>
+      </c>
+      <c r="C93" t="s">
         <v>163</v>
-      </c>
-      <c r="E93" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>122</v>
       </c>
-      <c r="D94" t="s">
+      <c r="B94" t="s">
+        <v>142</v>
+      </c>
+      <c r="C94" t="s">
         <v>164</v>
-      </c>
-      <c r="E94" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -3256,7 +3268,7 @@
         <v>122</v>
       </c>
       <c r="B95" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C95" t="s">
         <v>165</v>
@@ -3265,7 +3277,7 @@
         <v>165</v>
       </c>
       <c r="E95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -3273,7 +3285,7 @@
         <v>122</v>
       </c>
       <c r="B96" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C96" t="s">
         <v>167</v>
@@ -3282,7 +3294,7 @@
         <v>167</v>
       </c>
       <c r="E96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -3290,13 +3302,13 @@
         <v>122</v>
       </c>
       <c r="B97" t="s">
+        <v>170</v>
+      </c>
+      <c r="D97" t="s">
         <v>169</v>
       </c>
-      <c r="C97" t="s">
+      <c r="E97" t="s">
         <v>169</v>
-      </c>
-      <c r="E97" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -3304,13 +3316,13 @@
         <v>122</v>
       </c>
       <c r="B98" t="s">
+        <v>172</v>
+      </c>
+      <c r="D98" t="s">
         <v>171</v>
       </c>
-      <c r="C98" t="s">
+      <c r="E98" t="s">
         <v>171</v>
-      </c>
-      <c r="E98" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -3318,13 +3330,13 @@
         <v>122</v>
       </c>
       <c r="B99" t="s">
+        <v>174</v>
+      </c>
+      <c r="D99" t="s">
         <v>173</v>
       </c>
-      <c r="C99" t="s">
+      <c r="E99" t="s">
         <v>173</v>
-      </c>
-      <c r="E99" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -3332,13 +3344,13 @@
         <v>122</v>
       </c>
       <c r="B100" t="s">
+        <v>176</v>
+      </c>
+      <c r="D100" t="s">
         <v>175</v>
       </c>
-      <c r="C100" t="s">
+      <c r="E100" t="s">
         <v>175</v>
-      </c>
-      <c r="E100" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -3346,13 +3358,13 @@
         <v>122</v>
       </c>
       <c r="B101" t="s">
+        <v>178</v>
+      </c>
+      <c r="D101" t="s">
         <v>177</v>
       </c>
-      <c r="C101" t="s">
+      <c r="E101" t="s">
         <v>177</v>
-      </c>
-      <c r="E101" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -3360,13 +3372,13 @@
         <v>122</v>
       </c>
       <c r="B102" t="s">
+        <v>180</v>
+      </c>
+      <c r="D102" t="s">
         <v>179</v>
       </c>
-      <c r="C102" t="s">
+      <c r="E102" t="s">
         <v>179</v>
-      </c>
-      <c r="E102" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -3374,35 +3386,35 @@
         <v>122</v>
       </c>
       <c r="B103" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" t="s">
         <v>181</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>181</v>
-      </c>
-      <c r="E103" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>122</v>
       </c>
-      <c r="D104" t="s">
+      <c r="B104" t="s">
+        <v>184</v>
+      </c>
+      <c r="C104" t="s">
         <v>183</v>
-      </c>
-      <c r="E104" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>122</v>
       </c>
-      <c r="D105" t="s">
+      <c r="B105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C105" t="s">
         <v>185</v>
-      </c>
-      <c r="E105" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -3410,10 +3422,10 @@
         <v>122</v>
       </c>
       <c r="B106" t="s">
+        <v>166</v>
+      </c>
+      <c r="E106" t="s">
         <v>187</v>
-      </c>
-      <c r="E106" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -3421,10 +3433,10 @@
         <v>122</v>
       </c>
       <c r="B107" t="s">
+        <v>168</v>
+      </c>
+      <c r="E107" t="s">
         <v>188</v>
-      </c>
-      <c r="E107" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -3432,7 +3444,7 @@
         <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C108" t="s">
         <v>189</v>
@@ -3441,7 +3453,7 @@
         <v>189</v>
       </c>
       <c r="E108" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -3449,7 +3461,7 @@
         <v>122</v>
       </c>
       <c r="B109" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C109" t="s">
         <v>191</v>
@@ -3458,7 +3470,7 @@
         <v>191</v>
       </c>
       <c r="E109" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -3466,7 +3478,7 @@
         <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C110" t="s">
         <v>193</v>
@@ -3475,7 +3487,7 @@
         <v>193</v>
       </c>
       <c r="E110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -3483,7 +3495,7 @@
         <v>122</v>
       </c>
       <c r="B111" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C111" t="s">
         <v>195</v>
@@ -3492,7 +3504,7 @@
         <v>195</v>
       </c>
       <c r="E111" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -3500,13 +3512,13 @@
         <v>122</v>
       </c>
       <c r="B112" t="s">
+        <v>198</v>
+      </c>
+      <c r="D112" t="s">
         <v>197</v>
       </c>
-      <c r="C112" t="s">
+      <c r="E112" t="s">
         <v>197</v>
-      </c>
-      <c r="E112" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -3514,7 +3526,7 @@
         <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C113" t="s">
         <v>199</v>
@@ -3523,7 +3535,7 @@
         <v>199</v>
       </c>
       <c r="E113" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -3531,7 +3543,7 @@
         <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C114" t="s">
         <v>201</v>
@@ -3540,7 +3552,7 @@
         <v>201</v>
       </c>
       <c r="E114" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -3548,13 +3560,13 @@
         <v>122</v>
       </c>
       <c r="B115" t="s">
+        <v>204</v>
+      </c>
+      <c r="D115" t="s">
         <v>203</v>
       </c>
-      <c r="C115" t="s">
+      <c r="E115" t="s">
         <v>203</v>
-      </c>
-      <c r="E115" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -3562,46 +3574,46 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
+        <v>206</v>
+      </c>
+      <c r="C116" t="s">
         <v>205</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
         <v>205</v>
-      </c>
-      <c r="E116" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>122</v>
       </c>
-      <c r="D117" t="s">
+      <c r="B117" t="s">
+        <v>208</v>
+      </c>
+      <c r="C117" t="s">
         <v>207</v>
-      </c>
-      <c r="E117" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>122</v>
       </c>
-      <c r="D118" t="s">
+      <c r="B118" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" t="s">
         <v>209</v>
-      </c>
-      <c r="E118" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>122</v>
       </c>
-      <c r="D119" t="s">
+      <c r="B119" t="s">
+        <v>212</v>
+      </c>
+      <c r="C119" t="s">
         <v>211</v>
-      </c>
-      <c r="E119" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -3609,7 +3621,7 @@
         <v>5</v>
       </c>
       <c r="B120" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C120" t="s">
         <v>213</v>
@@ -3618,7 +3630,7 @@
         <v>213</v>
       </c>
       <c r="E120" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -3626,10 +3638,10 @@
         <v>5</v>
       </c>
       <c r="B121" t="s">
+        <v>216</v>
+      </c>
+      <c r="E121" t="s">
         <v>215</v>
-      </c>
-      <c r="E121" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -3637,10 +3649,10 @@
         <v>5</v>
       </c>
       <c r="B122" t="s">
+        <v>218</v>
+      </c>
+      <c r="E122" t="s">
         <v>217</v>
-      </c>
-      <c r="E122" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -3648,7 +3660,7 @@
         <v>5</v>
       </c>
       <c r="B123" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C123" t="s">
         <v>220</v>
@@ -3657,18 +3669,18 @@
         <v>220</v>
       </c>
       <c r="E123" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>5</v>
       </c>
-      <c r="D124" t="s">
+      <c r="B124" t="s">
+        <v>221</v>
+      </c>
+      <c r="C124" t="s">
         <v>222</v>
-      </c>
-      <c r="E124" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -3676,7 +3688,7 @@
         <v>5</v>
       </c>
       <c r="B125" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C125" t="s">
         <v>223</v>
@@ -3685,7 +3697,7 @@
         <v>223</v>
       </c>
       <c r="E125" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -3693,7 +3705,7 @@
         <v>5</v>
       </c>
       <c r="B126" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C126" t="s">
         <v>225</v>
@@ -3702,7 +3714,7 @@
         <v>225</v>
       </c>
       <c r="E126" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -3710,7 +3722,7 @@
         <v>5</v>
       </c>
       <c r="B127" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C127" t="s">
         <v>227</v>
@@ -3719,7 +3731,7 @@
         <v>227</v>
       </c>
       <c r="E127" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -3727,7 +3739,7 @@
         <v>5</v>
       </c>
       <c r="B128" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C128" t="s">
         <v>229</v>
@@ -3736,7 +3748,7 @@
         <v>229</v>
       </c>
       <c r="E128" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -3744,7 +3756,7 @@
         <v>5</v>
       </c>
       <c r="B129" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" t="s">
         <v>231</v>
@@ -3753,7 +3765,7 @@
         <v>231</v>
       </c>
       <c r="E129" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -3761,7 +3773,7 @@
         <v>5</v>
       </c>
       <c r="B130" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C130" t="s">
         <v>233</v>
@@ -3770,7 +3782,7 @@
         <v>233</v>
       </c>
       <c r="E130" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -3778,10 +3790,10 @@
         <v>5</v>
       </c>
       <c r="B131" t="s">
+        <v>236</v>
+      </c>
+      <c r="E131" t="s">
         <v>235</v>
-      </c>
-      <c r="E131" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3789,10 +3801,10 @@
         <v>5</v>
       </c>
       <c r="B132" t="s">
+        <v>238</v>
+      </c>
+      <c r="E132" t="s">
         <v>237</v>
-      </c>
-      <c r="E132" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3800,13 +3812,13 @@
         <v>5</v>
       </c>
       <c r="B133" t="s">
+        <v>241</v>
+      </c>
+      <c r="C133" t="s">
+        <v>240</v>
+      </c>
+      <c r="E133" t="s">
         <v>239</v>
-      </c>
-      <c r="D133" t="s">
-        <v>240</v>
-      </c>
-      <c r="E133" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3814,7 +3826,7 @@
         <v>5</v>
       </c>
       <c r="B134" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C134" t="s">
         <v>243</v>
@@ -3823,7 +3835,7 @@
         <v>243</v>
       </c>
       <c r="E134" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3831,10 +3843,10 @@
         <v>5</v>
       </c>
       <c r="B135" t="s">
+        <v>246</v>
+      </c>
+      <c r="E135" t="s">
         <v>245</v>
-      </c>
-      <c r="E135" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3842,27 +3854,27 @@
         <v>5</v>
       </c>
       <c r="B136" t="s">
+        <v>249</v>
+      </c>
+      <c r="C136" t="s">
+        <v>248</v>
+      </c>
+      <c r="D136" t="s">
         <v>247</v>
       </c>
-      <c r="C136" t="s">
+      <c r="E136" t="s">
         <v>247</v>
-      </c>
-      <c r="D136" t="s">
-        <v>248</v>
-      </c>
-      <c r="E136" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>5</v>
       </c>
-      <c r="D137" t="s">
+      <c r="B137" t="s">
+        <v>251</v>
+      </c>
+      <c r="C137" t="s">
         <v>250</v>
-      </c>
-      <c r="E137" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3870,13 +3882,13 @@
         <v>5</v>
       </c>
       <c r="B138" t="s">
+        <v>254</v>
+      </c>
+      <c r="D138" t="s">
+        <v>253</v>
+      </c>
+      <c r="E138" t="s">
         <v>252</v>
-      </c>
-      <c r="C138" t="s">
-        <v>253</v>
-      </c>
-      <c r="E138" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3884,13 +3896,13 @@
         <v>5</v>
       </c>
       <c r="B139" t="s">
+        <v>257</v>
+      </c>
+      <c r="D139" t="s">
+        <v>256</v>
+      </c>
+      <c r="E139" t="s">
         <v>255</v>
-      </c>
-      <c r="C139" t="s">
-        <v>256</v>
-      </c>
-      <c r="E139" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -3898,13 +3910,13 @@
         <v>5</v>
       </c>
       <c r="B140" t="s">
+        <v>259</v>
+      </c>
+      <c r="C140" t="s">
         <v>258</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" t="s">
         <v>258</v>
-      </c>
-      <c r="E140" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -3912,7 +3924,7 @@
         <v>5</v>
       </c>
       <c r="B141" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C141" t="s">
         <v>260</v>
@@ -3921,7 +3933,7 @@
         <v>260</v>
       </c>
       <c r="E141" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -3929,7 +3941,7 @@
         <v>5</v>
       </c>
       <c r="B142" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C142" t="s">
         <v>262</v>
@@ -3938,7 +3950,7 @@
         <v>262</v>
       </c>
       <c r="E142" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -3946,35 +3958,35 @@
         <v>5</v>
       </c>
       <c r="B143" t="s">
+        <v>265</v>
+      </c>
+      <c r="D143" t="s">
         <v>264</v>
       </c>
-      <c r="C143" t="s">
+      <c r="E143" t="s">
         <v>264</v>
-      </c>
-      <c r="E143" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>5</v>
       </c>
-      <c r="D144" t="s">
+      <c r="B144" t="s">
+        <v>267</v>
+      </c>
+      <c r="C144" t="s">
         <v>266</v>
-      </c>
-      <c r="E144" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>5</v>
       </c>
-      <c r="D145" t="s">
+      <c r="B145" t="s">
+        <v>269</v>
+      </c>
+      <c r="C145" t="s">
         <v>268</v>
-      </c>
-      <c r="E145" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3982,7 +3994,7 @@
         <v>5</v>
       </c>
       <c r="B146" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C146" t="s">
         <v>270</v>
@@ -3991,7 +4003,7 @@
         <v>270</v>
       </c>
       <c r="E146" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3999,16 +4011,16 @@
         <v>5</v>
       </c>
       <c r="B147" t="s">
+        <v>275</v>
+      </c>
+      <c r="C147" t="s">
+        <v>274</v>
+      </c>
+      <c r="D147" t="s">
+        <v>273</v>
+      </c>
+      <c r="E147" t="s">
         <v>272</v>
-      </c>
-      <c r="C147" t="s">
-        <v>273</v>
-      </c>
-      <c r="D147" t="s">
-        <v>274</v>
-      </c>
-      <c r="E147" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -4016,7 +4028,7 @@
         <v>5</v>
       </c>
       <c r="B148" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C148" t="s">
         <v>277</v>
@@ -4025,7 +4037,7 @@
         <v>277</v>
       </c>
       <c r="E148" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -4033,7 +4045,7 @@
         <v>5</v>
       </c>
       <c r="B149" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C149" t="s">
         <v>280</v>
@@ -4042,7 +4054,7 @@
         <v>280</v>
       </c>
       <c r="E149" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -4050,7 +4062,7 @@
         <v>5</v>
       </c>
       <c r="B150" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C150" t="s">
         <v>282</v>
@@ -4059,18 +4071,18 @@
         <v>282</v>
       </c>
       <c r="E150" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>5</v>
       </c>
-      <c r="C151" t="s">
+      <c r="B151" t="s">
+        <v>285</v>
+      </c>
+      <c r="D151" t="s">
         <v>284</v>
-      </c>
-      <c r="E151" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -4078,10 +4090,10 @@
         <v>5</v>
       </c>
       <c r="B152" t="s">
+        <v>287</v>
+      </c>
+      <c r="E152" t="s">
         <v>286</v>
-      </c>
-      <c r="E152" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -4089,10 +4101,10 @@
         <v>5</v>
       </c>
       <c r="B153" t="s">
+        <v>289</v>
+      </c>
+      <c r="E153" t="s">
         <v>288</v>
-      </c>
-      <c r="E153" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -4100,10 +4112,10 @@
         <v>5</v>
       </c>
       <c r="B154" t="s">
+        <v>291</v>
+      </c>
+      <c r="E154" t="s">
         <v>290</v>
-      </c>
-      <c r="E154" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -4111,10 +4123,10 @@
         <v>5</v>
       </c>
       <c r="B155" t="s">
+        <v>293</v>
+      </c>
+      <c r="E155" t="s">
         <v>292</v>
-      </c>
-      <c r="E155" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -4122,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="B156" t="s">
+        <v>295</v>
+      </c>
+      <c r="E156" t="s">
         <v>294</v>
-      </c>
-      <c r="E156" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -4133,15 +4145,15 @@
         <v>5</v>
       </c>
       <c r="B157" t="s">
+        <v>297</v>
+      </c>
+      <c r="E157" t="s">
         <v>296</v>
-      </c>
-      <c r="E157" t="s">
-        <v>297</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update lab_info data (procalcitonin, coagulation profile)
</commit_message>
<xml_diff>
--- a/lab_info.xlsx
+++ b/lab_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bigdata\my_packages\labbinder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BigData\mylib\labbinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31845ED9-70B2-47DF-B234-D6D1F45C4A93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7995D-1D31-4712-986E-3499CD75CDF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="319">
   <si>
     <t>sort1</t>
   </si>
@@ -917,6 +917,76 @@
   </si>
   <si>
     <t>HbA1c</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fibrinogen</t>
+  </si>
+  <si>
+    <t>FDP 정량</t>
+  </si>
+  <si>
+    <t>Anti-thrombin III</t>
+  </si>
+  <si>
+    <t>T3 (Triiodothyronine)</t>
+  </si>
+  <si>
+    <t>T3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fibrinogen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FDP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-dimer [정량]</t>
+  </si>
+  <si>
+    <t>d_dimer</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amylase</t>
+  </si>
+  <si>
+    <t>Lipase</t>
+  </si>
+  <si>
+    <t>NH3 (Ammonia)</t>
+  </si>
+  <si>
+    <t>Procalcitonin</t>
+  </si>
+  <si>
+    <t>ADA (Adenosine Deaminase), Blood</t>
+  </si>
+  <si>
+    <t>amylase</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lipase</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ammonia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>procalcitonin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADA</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -924,7 +994,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1092,6 +1162,12 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1519,12 +1595,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1881,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2577,16 +2656,10 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" t="s">
-        <v>78</v>
+        <v>303</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>302</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -2594,16 +2667,16 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2611,10 +2684,16 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2622,13 +2701,10 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2636,13 +2712,13 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -2650,16 +2726,13 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>298</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
-      </c>
-      <c r="D47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -2667,13 +2740,16 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>298</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>85</v>
       </c>
       <c r="E48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2681,13 +2757,13 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
       </c>
       <c r="E49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -2695,16 +2771,13 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -2712,13 +2785,16 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="D51" t="s">
+        <v>91</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2726,13 +2802,13 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2740,10 +2816,13 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>96</v>
       </c>
       <c r="E53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2751,10 +2830,10 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2762,10 +2841,10 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2773,10 +2852,10 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2784,10 +2863,10 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2795,10 +2874,10 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2806,10 +2885,10 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2817,10 +2896,10 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E60" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2828,10 +2907,10 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E61" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2839,10 +2918,10 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2850,10 +2929,10 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E63" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2861,10 +2940,10 @@
         <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2872,10 +2951,10 @@
         <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E65" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2883,10 +2962,10 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E66" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2894,10 +2973,10 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E67" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2905,10 +2984,10 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2916,27 +2995,21 @@
         <v>5</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>123</v>
-      </c>
-      <c r="C70" t="s">
-        <v>106</v>
-      </c>
-      <c r="D70" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E70" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2944,13 +3017,16 @@
         <v>122</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>106</v>
+      </c>
+      <c r="D71" t="s">
+        <v>107</v>
       </c>
       <c r="E71" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -2958,16 +3034,13 @@
         <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C72" t="s">
-        <v>127</v>
-      </c>
-      <c r="D72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E72" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2975,16 +3048,16 @@
         <v>122</v>
       </c>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C73" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D73" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E73" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2992,16 +3065,16 @@
         <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -3009,16 +3082,16 @@
         <v>122</v>
       </c>
       <c r="B75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="D75" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="E75" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -3026,10 +3099,16 @@
         <v>122</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C76" t="s">
-        <v>134</v>
+        <v>26</v>
+      </c>
+      <c r="D76" t="s">
+        <v>26</v>
+      </c>
+      <c r="E76" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -3037,16 +3116,10 @@
         <v>122</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
-      </c>
-      <c r="D77" t="s">
-        <v>136</v>
-      </c>
-      <c r="E77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -3054,16 +3127,16 @@
         <v>122</v>
       </c>
       <c r="B78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -3071,16 +3144,16 @@
         <v>122</v>
       </c>
       <c r="B79" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C79" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D79" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E79" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -3088,16 +3161,16 @@
         <v>122</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D80" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E80" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -3105,16 +3178,16 @@
         <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D81" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E81" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -3122,10 +3195,16 @@
         <v>122</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="C82" t="s">
+        <v>147</v>
       </c>
       <c r="D82" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="E82" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -3133,10 +3212,10 @@
         <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D83" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -3144,13 +3223,10 @@
         <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D84" t="s">
-        <v>153</v>
-      </c>
-      <c r="E84" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -3158,10 +3234,13 @@
         <v>122</v>
       </c>
       <c r="B85" t="s">
-        <v>123</v>
-      </c>
-      <c r="C85" t="s">
-        <v>155</v>
+        <v>154</v>
+      </c>
+      <c r="D85" t="s">
+        <v>153</v>
+      </c>
+      <c r="E85" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -3169,10 +3248,10 @@
         <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -3180,10 +3259,10 @@
         <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C87" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -3191,10 +3270,10 @@
         <v>122</v>
       </c>
       <c r="B88" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C88" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -3202,10 +3281,10 @@
         <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -3213,10 +3292,10 @@
         <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -3224,10 +3303,10 @@
         <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C91" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -3235,10 +3314,10 @@
         <v>122</v>
       </c>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C92" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -3246,10 +3325,10 @@
         <v>122</v>
       </c>
       <c r="B93" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -3257,10 +3336,10 @@
         <v>122</v>
       </c>
       <c r="B94" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -3268,16 +3347,10 @@
         <v>122</v>
       </c>
       <c r="B95" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>165</v>
-      </c>
-      <c r="D95" t="s">
-        <v>165</v>
-      </c>
-      <c r="E95" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -3285,16 +3358,16 @@
         <v>122</v>
       </c>
       <c r="B96" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C96" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D96" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E96" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -3302,13 +3375,16 @@
         <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>170</v>
+        <v>168</v>
+      </c>
+      <c r="C97" t="s">
+        <v>167</v>
       </c>
       <c r="D97" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E97" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -3316,13 +3392,13 @@
         <v>122</v>
       </c>
       <c r="B98" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D98" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E98" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -3330,13 +3406,13 @@
         <v>122</v>
       </c>
       <c r="B99" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D99" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -3344,13 +3420,13 @@
         <v>122</v>
       </c>
       <c r="B100" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D100" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E100" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -3358,13 +3434,13 @@
         <v>122</v>
       </c>
       <c r="B101" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D101" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E101" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -3372,13 +3448,13 @@
         <v>122</v>
       </c>
       <c r="B102" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -3386,13 +3462,13 @@
         <v>122</v>
       </c>
       <c r="B103" t="s">
-        <v>182</v>
-      </c>
-      <c r="C103" t="s">
-        <v>181</v>
+        <v>180</v>
+      </c>
+      <c r="D103" t="s">
+        <v>179</v>
       </c>
       <c r="E103" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -3400,10 +3476,13 @@
         <v>122</v>
       </c>
       <c r="B104" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C104" t="s">
-        <v>183</v>
+        <v>181</v>
+      </c>
+      <c r="E104" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -3411,10 +3490,10 @@
         <v>122</v>
       </c>
       <c r="B105" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C105" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -3422,10 +3501,10 @@
         <v>122</v>
       </c>
       <c r="B106" t="s">
-        <v>166</v>
-      </c>
-      <c r="E106" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="C106" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -3433,10 +3512,10 @@
         <v>122</v>
       </c>
       <c r="B107" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E107" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -3444,16 +3523,10 @@
         <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>190</v>
-      </c>
-      <c r="C108" t="s">
-        <v>189</v>
-      </c>
-      <c r="D108" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="E108" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -3461,16 +3534,16 @@
         <v>122</v>
       </c>
       <c r="B109" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C109" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D109" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E109" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -3478,16 +3551,16 @@
         <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C110" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D110" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E110" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -3495,16 +3568,16 @@
         <v>122</v>
       </c>
       <c r="B111" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C111" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D111" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E111" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -3512,13 +3585,16 @@
         <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>198</v>
+        <v>196</v>
+      </c>
+      <c r="C112" t="s">
+        <v>195</v>
       </c>
       <c r="D112" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E112" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -3526,16 +3602,13 @@
         <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>200</v>
-      </c>
-      <c r="C113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D113" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E113" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -3543,16 +3616,16 @@
         <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D114" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E114" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -3560,13 +3633,16 @@
         <v>122</v>
       </c>
       <c r="B115" t="s">
-        <v>204</v>
+        <v>202</v>
+      </c>
+      <c r="C115" t="s">
+        <v>201</v>
       </c>
       <c r="D115" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E115" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -3574,13 +3650,13 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>206</v>
-      </c>
-      <c r="C116" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="D116" t="s">
+        <v>203</v>
       </c>
       <c r="E116" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -3588,10 +3664,13 @@
         <v>122</v>
       </c>
       <c r="B117" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C117" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E117" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -3599,10 +3678,10 @@
         <v>122</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C118" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -3610,27 +3689,21 @@
         <v>122</v>
       </c>
       <c r="B119" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C119" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C120" t="s">
-        <v>213</v>
-      </c>
-      <c r="D120" t="s">
-        <v>213</v>
-      </c>
-      <c r="E120" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -3638,10 +3711,16 @@
         <v>5</v>
       </c>
       <c r="B121" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+      <c r="C121" t="s">
+        <v>213</v>
+      </c>
+      <c r="D121" t="s">
+        <v>213</v>
       </c>
       <c r="E121" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -3649,10 +3728,10 @@
         <v>5</v>
       </c>
       <c r="B122" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E122" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -3660,16 +3739,10 @@
         <v>5</v>
       </c>
       <c r="B123" t="s">
-        <v>221</v>
-      </c>
-      <c r="C123" t="s">
-        <v>220</v>
-      </c>
-      <c r="D123" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E123" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -3680,7 +3753,13 @@
         <v>221</v>
       </c>
       <c r="C124" t="s">
-        <v>222</v>
+        <v>220</v>
+      </c>
+      <c r="D124" t="s">
+        <v>220</v>
+      </c>
+      <c r="E124" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -3688,16 +3767,10 @@
         <v>5</v>
       </c>
       <c r="B125" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C125" t="s">
-        <v>223</v>
-      </c>
-      <c r="D125" t="s">
-        <v>223</v>
-      </c>
-      <c r="E125" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -3705,16 +3778,16 @@
         <v>5</v>
       </c>
       <c r="B126" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C126" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D126" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E126" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -3722,16 +3795,16 @@
         <v>5</v>
       </c>
       <c r="B127" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C127" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D127" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E127" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -3739,16 +3812,16 @@
         <v>5</v>
       </c>
       <c r="B128" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C128" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D128" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E128" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -3756,16 +3829,16 @@
         <v>5</v>
       </c>
       <c r="B129" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C129" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D129" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E129" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -3773,16 +3846,16 @@
         <v>5</v>
       </c>
       <c r="B130" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C130" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D130" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E130" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -3790,10 +3863,16 @@
         <v>5</v>
       </c>
       <c r="B131" t="s">
-        <v>236</v>
+        <v>234</v>
+      </c>
+      <c r="C131" t="s">
+        <v>233</v>
+      </c>
+      <c r="D131" t="s">
+        <v>233</v>
       </c>
       <c r="E131" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3801,10 +3880,10 @@
         <v>5</v>
       </c>
       <c r="B132" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E132" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3812,13 +3891,10 @@
         <v>5</v>
       </c>
       <c r="B133" t="s">
-        <v>241</v>
-      </c>
-      <c r="C133" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E133" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3826,16 +3902,13 @@
         <v>5</v>
       </c>
       <c r="B134" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C134" t="s">
-        <v>243</v>
-      </c>
-      <c r="D134" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E134" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3843,10 +3916,16 @@
         <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>246</v>
+        <v>244</v>
+      </c>
+      <c r="C135" t="s">
+        <v>243</v>
+      </c>
+      <c r="D135" t="s">
+        <v>243</v>
       </c>
       <c r="E135" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3854,16 +3933,10 @@
         <v>5</v>
       </c>
       <c r="B136" t="s">
-        <v>249</v>
-      </c>
-      <c r="C136" t="s">
-        <v>248</v>
-      </c>
-      <c r="D136" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E136" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3871,10 +3944,16 @@
         <v>5</v>
       </c>
       <c r="B137" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C137" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+      <c r="D137" t="s">
+        <v>247</v>
+      </c>
+      <c r="E137" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3882,13 +3961,10 @@
         <v>5</v>
       </c>
       <c r="B138" t="s">
-        <v>254</v>
-      </c>
-      <c r="D138" t="s">
-        <v>253</v>
-      </c>
-      <c r="E138" t="s">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="C138" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3896,13 +3972,13 @@
         <v>5</v>
       </c>
       <c r="B139" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D139" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E139" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -3910,13 +3986,13 @@
         <v>5</v>
       </c>
       <c r="B140" t="s">
-        <v>259</v>
-      </c>
-      <c r="C140" t="s">
-        <v>258</v>
+        <v>257</v>
+      </c>
+      <c r="D140" t="s">
+        <v>256</v>
       </c>
       <c r="E140" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -3924,16 +4000,13 @@
         <v>5</v>
       </c>
       <c r="B141" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C141" t="s">
-        <v>260</v>
-      </c>
-      <c r="D141" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E141" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -3941,16 +4014,16 @@
         <v>5</v>
       </c>
       <c r="B142" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -3958,13 +4031,16 @@
         <v>5</v>
       </c>
       <c r="B143" t="s">
-        <v>265</v>
+        <v>263</v>
+      </c>
+      <c r="C143" t="s">
+        <v>262</v>
       </c>
       <c r="D143" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E143" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -3972,10 +4048,13 @@
         <v>5</v>
       </c>
       <c r="B144" t="s">
-        <v>267</v>
-      </c>
-      <c r="C144" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="D144" t="s">
+        <v>264</v>
+      </c>
+      <c r="E144" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -3983,10 +4062,10 @@
         <v>5</v>
       </c>
       <c r="B145" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C145" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3994,16 +4073,10 @@
         <v>5</v>
       </c>
       <c r="B146" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C146" t="s">
-        <v>270</v>
-      </c>
-      <c r="D146" t="s">
-        <v>270</v>
-      </c>
-      <c r="E146" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -4011,16 +4084,16 @@
         <v>5</v>
       </c>
       <c r="B147" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C147" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D147" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E147" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -4028,16 +4101,16 @@
         <v>5</v>
       </c>
       <c r="B148" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C148" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D148" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E148" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -4045,16 +4118,16 @@
         <v>5</v>
       </c>
       <c r="B149" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C149" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D149" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E149" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -4062,16 +4135,16 @@
         <v>5</v>
       </c>
       <c r="B150" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C150" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D150" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E150" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -4079,10 +4152,16 @@
         <v>5</v>
       </c>
       <c r="B151" t="s">
-        <v>285</v>
+        <v>283</v>
+      </c>
+      <c r="C151" t="s">
+        <v>282</v>
       </c>
       <c r="D151" t="s">
-        <v>284</v>
+        <v>282</v>
+      </c>
+      <c r="E151" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -4090,10 +4169,10 @@
         <v>5</v>
       </c>
       <c r="B152" t="s">
-        <v>287</v>
-      </c>
-      <c r="E152" t="s">
-        <v>286</v>
+        <v>285</v>
+      </c>
+      <c r="D152" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -4101,10 +4180,10 @@
         <v>5</v>
       </c>
       <c r="B153" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E153" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -4112,10 +4191,10 @@
         <v>5</v>
       </c>
       <c r="B154" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E154" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -4123,10 +4202,10 @@
         <v>5</v>
       </c>
       <c r="B155" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E155" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -4134,10 +4213,10 @@
         <v>5</v>
       </c>
       <c r="B156" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E156" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -4145,10 +4224,120 @@
         <v>5</v>
       </c>
       <c r="B157" t="s">
+        <v>295</v>
+      </c>
+      <c r="E157" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158" t="s">
         <v>297</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E158" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" t="s">
+        <v>304</v>
+      </c>
+      <c r="E159" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" t="s">
+        <v>305</v>
+      </c>
+      <c r="E160" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>306</v>
+      </c>
+      <c r="E161" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" t="s">
+        <v>308</v>
+      </c>
+      <c r="E162" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" t="s">
+        <v>314</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" t="s">
+        <v>315</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" t="s">
+        <v>316</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" t="s">
+        <v>317</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" t="s">
+        <v>318</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lab_info (lympho, neutro, etc...)
</commit_message>
<xml_diff>
--- a/lab_info.xlsx
+++ b/lab_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BigData\mylib\labbinder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bigdata\mylib\labbinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7995D-1D31-4712-986E-3499CD75CDF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA7CAC8-B26E-4148-86C9-18726D157B9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="334">
   <si>
     <t>sort1</t>
   </si>
@@ -987,6 +987,56 @@
   </si>
   <si>
     <t>ADA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lymphocyte</t>
+  </si>
+  <si>
+    <t>Monocytes</t>
+  </si>
+  <si>
+    <t>Neutrophil</t>
+  </si>
+  <si>
+    <t>Eosinophil</t>
+  </si>
+  <si>
+    <t>Basophil</t>
+  </si>
+  <si>
+    <t>Atypical Lymphocyte %</t>
+  </si>
+  <si>
+    <t>Band Neutrophil %</t>
+  </si>
+  <si>
+    <t>Metamyelocyte %</t>
+  </si>
+  <si>
+    <t>Myelocyte %</t>
+  </si>
+  <si>
+    <t>Blast %</t>
+  </si>
+  <si>
+    <t>aty_lympho_percent</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>band_neutro_percent</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>metamyelo_percent</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>myelo_percent</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blast_percent</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1595,7 +1645,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1604,6 +1654,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1960,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4340,6 +4393,116 @@
         <v>313</v>
       </c>
     </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update lab_info (change variable name)
</commit_message>
<xml_diff>
--- a/lab_info.xlsx
+++ b/lab_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bigdata\mylib\labbinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA7CAC8-B26E-4148-86C9-18726D157B9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F29EB1-A90E-4AA2-BFDC-F84830F557B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="339">
   <si>
     <t>sort1</t>
   </si>
@@ -1020,23 +1020,43 @@
     <t>Blast %</t>
   </si>
   <si>
-    <t>aty_lympho_percent</t>
+    <t>basophil</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>band_neutro_percent</t>
+    <t>eosinophil</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>metamyelo_percent</t>
+    <t>neutrophil</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>myelo_percent</t>
+    <t>monocytes</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>blast_percent</t>
+    <t>lymphocyte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aty_lympho_pct</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>band_neutro_pct</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>metamyelo_pct</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>myelo_pct</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blast_pct</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2015,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C174" sqref="C174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2250,164 +2270,110 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
+      <c r="B14" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
+      <c r="B15" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
+      <c r="B16" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
+      <c r="B17" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" t="s">
-        <v>30</v>
+      <c r="B18" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
-        <v>32</v>
+      <c r="B19" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
+      <c r="B20" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>36</v>
+      <c r="B21" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
+      <c r="B22" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
+      <c r="B23" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2415,16 +2381,16 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2432,16 +2398,16 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2449,16 +2415,16 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2466,16 +2432,16 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2483,16 +2449,16 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2500,16 +2466,10 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2517,16 +2477,16 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2534,16 +2494,16 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -2551,16 +2511,16 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -2568,16 +2528,16 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -2585,16 +2545,16 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2602,16 +2562,16 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -2619,16 +2579,16 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -2636,10 +2596,16 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
       </c>
       <c r="E37" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2647,10 +2613,16 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -2658,16 +2630,16 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E39" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -2675,16 +2647,16 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -2692,16 +2664,16 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -2709,10 +2681,16 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>303</v>
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>302</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -2720,16 +2698,16 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2737,16 +2715,16 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2754,10 +2732,16 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>63</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2765,13 +2749,16 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -2779,13 +2766,10 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -2793,16 +2777,10 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>298</v>
-      </c>
-      <c r="C48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2810,13 +2788,16 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>71</v>
+      </c>
+      <c r="D49" t="s">
+        <v>71</v>
       </c>
       <c r="E49" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -2824,13 +2805,16 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="C50" t="s">
+        <v>74</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E50" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -2838,16 +2822,16 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E51" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2855,13 +2839,10 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" t="s">
-        <v>94</v>
+        <v>303</v>
       </c>
       <c r="E52" t="s">
-        <v>93</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2869,13 +2850,16 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>78</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
       </c>
       <c r="E53" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2883,10 +2867,16 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" t="s">
+        <v>79</v>
       </c>
       <c r="E54" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2894,10 +2884,10 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2905,10 +2895,13 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="C56" t="s">
+        <v>83</v>
       </c>
       <c r="E56" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2916,10 +2909,13 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>84</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2927,10 +2923,16 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>298</v>
+      </c>
+      <c r="C58" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" t="s">
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2938,10 +2940,13 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="C59" t="s">
+        <v>87</v>
       </c>
       <c r="E59" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,10 +2954,13 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>111</v>
+        <v>90</v>
+      </c>
+      <c r="D60" t="s">
+        <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2960,10 +2968,16 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>92</v>
+      </c>
+      <c r="C61" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" t="s">
+        <v>91</v>
       </c>
       <c r="E61" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2971,10 +2985,13 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>95</v>
+      </c>
+      <c r="C62" t="s">
+        <v>94</v>
       </c>
       <c r="E62" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2982,10 +2999,13 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
+        <v>97</v>
+      </c>
+      <c r="C63" t="s">
+        <v>96</v>
       </c>
       <c r="E63" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2993,10 +3013,10 @@
         <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -3004,10 +3024,10 @@
         <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -3015,10 +3035,10 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E66" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -3026,10 +3046,10 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E67" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -3037,10 +3057,10 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E68" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -3048,10 +3068,10 @@
         <v>5</v>
       </c>
       <c r="B69" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E69" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -3059,171 +3079,120 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E70" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B71" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71" t="s">
-        <v>106</v>
-      </c>
-      <c r="D71" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>124</v>
-      </c>
-      <c r="C72" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E72" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
-        <v>128</v>
-      </c>
-      <c r="C73" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E73" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" t="s">
-        <v>129</v>
-      </c>
-      <c r="D74" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="E74" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
-      </c>
-      <c r="C75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="E75" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>133</v>
-      </c>
-      <c r="C76" t="s">
-        <v>26</v>
-      </c>
-      <c r="D76" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="E76" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
-      </c>
-      <c r="C77" t="s">
-        <v>134</v>
+        <v>115</v>
+      </c>
+      <c r="E77" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
-      </c>
-      <c r="C78" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="E78" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>139</v>
-      </c>
-      <c r="C79" t="s">
-        <v>138</v>
-      </c>
-      <c r="D79" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="E79" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>142</v>
-      </c>
-      <c r="C80" t="s">
-        <v>141</v>
-      </c>
-      <c r="D80" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="E80" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -3231,16 +3200,16 @@
         <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C81" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="D81" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -3248,16 +3217,13 @@
         <v>122</v>
       </c>
       <c r="B82" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C82" t="s">
-        <v>147</v>
-      </c>
-      <c r="D82" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E82" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -3265,10 +3231,16 @@
         <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>150</v>
+        <v>128</v>
+      </c>
+      <c r="C83" t="s">
+        <v>127</v>
       </c>
       <c r="D83" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="E83" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -3276,10 +3248,16 @@
         <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>152</v>
+        <v>130</v>
+      </c>
+      <c r="C84" t="s">
+        <v>129</v>
       </c>
       <c r="D84" t="s">
-        <v>151</v>
+        <v>129</v>
+      </c>
+      <c r="E84" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -3287,13 +3265,16 @@
         <v>122</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>132</v>
+      </c>
+      <c r="C85" t="s">
+        <v>131</v>
       </c>
       <c r="D85" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="E85" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -3301,10 +3282,16 @@
         <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C86" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="D86" t="s">
+        <v>26</v>
+      </c>
+      <c r="E86" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -3312,10 +3299,10 @@
         <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C87" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -3323,10 +3310,16 @@
         <v>122</v>
       </c>
       <c r="B88" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C88" t="s">
-        <v>157</v>
+        <v>136</v>
+      </c>
+      <c r="D88" t="s">
+        <v>136</v>
+      </c>
+      <c r="E88" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -3334,10 +3327,16 @@
         <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C89" t="s">
-        <v>158</v>
+        <v>138</v>
+      </c>
+      <c r="D89" t="s">
+        <v>138</v>
+      </c>
+      <c r="E89" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -3345,10 +3344,16 @@
         <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>159</v>
+        <v>141</v>
+      </c>
+      <c r="D90" t="s">
+        <v>140</v>
+      </c>
+      <c r="E90" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -3356,10 +3361,16 @@
         <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C91" t="s">
-        <v>160</v>
+        <v>144</v>
+      </c>
+      <c r="D91" t="s">
+        <v>143</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -3367,10 +3378,16 @@
         <v>122</v>
       </c>
       <c r="B92" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C92" t="s">
-        <v>161</v>
+        <v>147</v>
+      </c>
+      <c r="D92" t="s">
+        <v>146</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -3378,10 +3395,10 @@
         <v>122</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
-      </c>
-      <c r="C93" t="s">
-        <v>162</v>
+        <v>150</v>
+      </c>
+      <c r="D93" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -3389,10 +3406,10 @@
         <v>122</v>
       </c>
       <c r="B94" t="s">
-        <v>139</v>
-      </c>
-      <c r="C94" t="s">
-        <v>163</v>
+        <v>152</v>
+      </c>
+      <c r="D94" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -3400,10 +3417,13 @@
         <v>122</v>
       </c>
       <c r="B95" t="s">
-        <v>142</v>
-      </c>
-      <c r="C95" t="s">
-        <v>164</v>
+        <v>154</v>
+      </c>
+      <c r="D95" t="s">
+        <v>153</v>
+      </c>
+      <c r="E95" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -3411,16 +3431,10 @@
         <v>122</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="C96" t="s">
-        <v>165</v>
-      </c>
-      <c r="D96" t="s">
-        <v>165</v>
-      </c>
-      <c r="E96" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -3428,16 +3442,10 @@
         <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="C97" t="s">
-        <v>167</v>
-      </c>
-      <c r="D97" t="s">
-        <v>167</v>
-      </c>
-      <c r="E97" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -3445,13 +3453,10 @@
         <v>122</v>
       </c>
       <c r="B98" t="s">
-        <v>170</v>
-      </c>
-      <c r="D98" t="s">
-        <v>169</v>
-      </c>
-      <c r="E98" t="s">
-        <v>169</v>
+        <v>128</v>
+      </c>
+      <c r="C98" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -3459,13 +3464,10 @@
         <v>122</v>
       </c>
       <c r="B99" t="s">
-        <v>172</v>
-      </c>
-      <c r="D99" t="s">
-        <v>171</v>
-      </c>
-      <c r="E99" t="s">
-        <v>171</v>
+        <v>130</v>
+      </c>
+      <c r="C99" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -3473,13 +3475,10 @@
         <v>122</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
-      </c>
-      <c r="D100" t="s">
-        <v>173</v>
-      </c>
-      <c r="E100" t="s">
-        <v>173</v>
+        <v>132</v>
+      </c>
+      <c r="C100" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -3487,13 +3486,10 @@
         <v>122</v>
       </c>
       <c r="B101" t="s">
-        <v>176</v>
-      </c>
-      <c r="D101" t="s">
-        <v>175</v>
-      </c>
-      <c r="E101" t="s">
-        <v>175</v>
+        <v>133</v>
+      </c>
+      <c r="C101" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -3501,13 +3497,10 @@
         <v>122</v>
       </c>
       <c r="B102" t="s">
-        <v>178</v>
-      </c>
-      <c r="D102" t="s">
-        <v>177</v>
-      </c>
-      <c r="E102" t="s">
-        <v>177</v>
+        <v>135</v>
+      </c>
+      <c r="C102" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -3515,13 +3508,10 @@
         <v>122</v>
       </c>
       <c r="B103" t="s">
-        <v>180</v>
-      </c>
-      <c r="D103" t="s">
-        <v>179</v>
-      </c>
-      <c r="E103" t="s">
-        <v>179</v>
+        <v>137</v>
+      </c>
+      <c r="C103" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -3529,13 +3519,10 @@
         <v>122</v>
       </c>
       <c r="B104" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="C104" t="s">
-        <v>181</v>
-      </c>
-      <c r="E104" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -3543,10 +3530,10 @@
         <v>122</v>
       </c>
       <c r="B105" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="C105" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -3554,10 +3541,16 @@
         <v>122</v>
       </c>
       <c r="B106" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>165</v>
+      </c>
+      <c r="D106" t="s">
+        <v>165</v>
+      </c>
+      <c r="E106" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -3565,10 +3558,16 @@
         <v>122</v>
       </c>
       <c r="B107" t="s">
-        <v>166</v>
+        <v>168</v>
+      </c>
+      <c r="C107" t="s">
+        <v>167</v>
+      </c>
+      <c r="D107" t="s">
+        <v>167</v>
       </c>
       <c r="E107" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -3576,10 +3575,13 @@
         <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>168</v>
+        <v>170</v>
+      </c>
+      <c r="D108" t="s">
+        <v>169</v>
       </c>
       <c r="E108" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -3587,16 +3589,13 @@
         <v>122</v>
       </c>
       <c r="B109" t="s">
-        <v>190</v>
-      </c>
-      <c r="C109" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="D109" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -3604,16 +3603,13 @@
         <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>192</v>
-      </c>
-      <c r="C110" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D110" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E110" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -3621,16 +3617,13 @@
         <v>122</v>
       </c>
       <c r="B111" t="s">
-        <v>194</v>
-      </c>
-      <c r="C111" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="D111" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="E111" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -3638,16 +3631,13 @@
         <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>196</v>
-      </c>
-      <c r="C112" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D112" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="E112" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -3655,13 +3645,13 @@
         <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D113" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E113" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -3669,16 +3659,13 @@
         <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C114" t="s">
-        <v>199</v>
-      </c>
-      <c r="D114" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E114" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -3686,16 +3673,10 @@
         <v>122</v>
       </c>
       <c r="B115" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="C115" t="s">
-        <v>201</v>
-      </c>
-      <c r="D115" t="s">
-        <v>201</v>
-      </c>
-      <c r="E115" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -3703,13 +3684,10 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>204</v>
-      </c>
-      <c r="D116" t="s">
-        <v>203</v>
-      </c>
-      <c r="E116" t="s">
-        <v>203</v>
+        <v>186</v>
+      </c>
+      <c r="C116" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -3717,13 +3695,10 @@
         <v>122</v>
       </c>
       <c r="B117" t="s">
-        <v>206</v>
-      </c>
-      <c r="C117" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="E117" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -3731,10 +3706,10 @@
         <v>122</v>
       </c>
       <c r="B118" t="s">
-        <v>208</v>
-      </c>
-      <c r="C118" t="s">
-        <v>207</v>
+        <v>168</v>
+      </c>
+      <c r="E118" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -3742,10 +3717,16 @@
         <v>122</v>
       </c>
       <c r="B119" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C119" t="s">
-        <v>209</v>
+        <v>189</v>
+      </c>
+      <c r="D119" t="s">
+        <v>189</v>
+      </c>
+      <c r="E119" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -3753,162 +3734,159 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C120" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="D120" t="s">
+        <v>191</v>
+      </c>
+      <c r="E120" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C121" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D121" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="E121" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>216</v>
+        <v>196</v>
+      </c>
+      <c r="C122" t="s">
+        <v>195</v>
+      </c>
+      <c r="D122" t="s">
+        <v>195</v>
       </c>
       <c r="E122" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>218</v>
+        <v>198</v>
+      </c>
+      <c r="D123" t="s">
+        <v>197</v>
       </c>
       <c r="E123" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="C124" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="D124" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="E124" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="C125" t="s">
-        <v>222</v>
+        <v>201</v>
+      </c>
+      <c r="D125" t="s">
+        <v>201</v>
+      </c>
+      <c r="E125" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>224</v>
-      </c>
-      <c r="C126" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="D126" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="E126" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="C127" t="s">
-        <v>225</v>
-      </c>
-      <c r="D127" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="E127" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B128" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="C128" t="s">
-        <v>227</v>
-      </c>
-      <c r="D128" t="s">
-        <v>227</v>
-      </c>
-      <c r="E128" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B129" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C129" t="s">
-        <v>229</v>
-      </c>
-      <c r="D129" t="s">
-        <v>229</v>
-      </c>
-      <c r="E129" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B130" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C130" t="s">
-        <v>231</v>
-      </c>
-      <c r="D130" t="s">
-        <v>231</v>
-      </c>
-      <c r="E130" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -3916,16 +3894,16 @@
         <v>5</v>
       </c>
       <c r="B131" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C131" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="D131" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="E131" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3933,10 +3911,10 @@
         <v>5</v>
       </c>
       <c r="B132" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="E132" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3944,10 +3922,10 @@
         <v>5</v>
       </c>
       <c r="B133" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="E133" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3955,13 +3933,16 @@
         <v>5</v>
       </c>
       <c r="B134" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C134" t="s">
-        <v>240</v>
+        <v>220</v>
+      </c>
+      <c r="D134" t="s">
+        <v>220</v>
       </c>
       <c r="E134" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3969,16 +3950,10 @@
         <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="C135" t="s">
-        <v>243</v>
-      </c>
-      <c r="D135" t="s">
-        <v>243</v>
-      </c>
-      <c r="E135" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3986,10 +3961,16 @@
         <v>5</v>
       </c>
       <c r="B136" t="s">
-        <v>246</v>
+        <v>224</v>
+      </c>
+      <c r="C136" t="s">
+        <v>223</v>
+      </c>
+      <c r="D136" t="s">
+        <v>223</v>
       </c>
       <c r="E136" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3997,16 +3978,16 @@
         <v>5</v>
       </c>
       <c r="B137" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="C137" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="D137" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="E137" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -4014,10 +3995,16 @@
         <v>5</v>
       </c>
       <c r="B138" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="C138" t="s">
-        <v>250</v>
+        <v>227</v>
+      </c>
+      <c r="D138" t="s">
+        <v>227</v>
+      </c>
+      <c r="E138" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -4025,13 +4012,16 @@
         <v>5</v>
       </c>
       <c r="B139" t="s">
-        <v>254</v>
+        <v>230</v>
+      </c>
+      <c r="C139" t="s">
+        <v>229</v>
       </c>
       <c r="D139" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E139" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -4039,13 +4029,16 @@
         <v>5</v>
       </c>
       <c r="B140" t="s">
-        <v>257</v>
+        <v>232</v>
+      </c>
+      <c r="C140" t="s">
+        <v>231</v>
       </c>
       <c r="D140" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="E140" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -4053,13 +4046,16 @@
         <v>5</v>
       </c>
       <c r="B141" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="C141" t="s">
-        <v>258</v>
+        <v>233</v>
+      </c>
+      <c r="D141" t="s">
+        <v>233</v>
       </c>
       <c r="E141" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -4067,16 +4063,10 @@
         <v>5</v>
       </c>
       <c r="B142" t="s">
-        <v>261</v>
-      </c>
-      <c r="C142" t="s">
-        <v>260</v>
-      </c>
-      <c r="D142" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="E142" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -4084,16 +4074,10 @@
         <v>5</v>
       </c>
       <c r="B143" t="s">
-        <v>263</v>
-      </c>
-      <c r="C143" t="s">
-        <v>262</v>
-      </c>
-      <c r="D143" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="E143" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -4101,13 +4085,13 @@
         <v>5</v>
       </c>
       <c r="B144" t="s">
-        <v>265</v>
-      </c>
-      <c r="D144" t="s">
-        <v>264</v>
+        <v>241</v>
+      </c>
+      <c r="C144" t="s">
+        <v>240</v>
       </c>
       <c r="E144" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -4115,10 +4099,16 @@
         <v>5</v>
       </c>
       <c r="B145" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="C145" t="s">
-        <v>266</v>
+        <v>243</v>
+      </c>
+      <c r="D145" t="s">
+        <v>243</v>
+      </c>
+      <c r="E145" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -4126,10 +4116,10 @@
         <v>5</v>
       </c>
       <c r="B146" t="s">
-        <v>269</v>
-      </c>
-      <c r="C146" t="s">
-        <v>268</v>
+        <v>246</v>
+      </c>
+      <c r="E146" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -4137,16 +4127,16 @@
         <v>5</v>
       </c>
       <c r="B147" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C147" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="D147" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="E147" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -4154,16 +4144,10 @@
         <v>5</v>
       </c>
       <c r="B148" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="C148" t="s">
-        <v>274</v>
-      </c>
-      <c r="D148" t="s">
-        <v>273</v>
-      </c>
-      <c r="E148" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -4171,16 +4155,13 @@
         <v>5</v>
       </c>
       <c r="B149" t="s">
-        <v>278</v>
-      </c>
-      <c r="C149" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="D149" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="E149" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -4188,16 +4169,13 @@
         <v>5</v>
       </c>
       <c r="B150" t="s">
-        <v>280</v>
-      </c>
-      <c r="C150" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="D150" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="E150" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -4205,16 +4183,13 @@
         <v>5</v>
       </c>
       <c r="B151" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="C151" t="s">
-        <v>282</v>
-      </c>
-      <c r="D151" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="E151" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -4222,10 +4197,16 @@
         <v>5</v>
       </c>
       <c r="B152" t="s">
-        <v>285</v>
+        <v>261</v>
+      </c>
+      <c r="C152" t="s">
+        <v>260</v>
       </c>
       <c r="D152" t="s">
-        <v>284</v>
+        <v>260</v>
+      </c>
+      <c r="E152" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -4233,10 +4214,16 @@
         <v>5</v>
       </c>
       <c r="B153" t="s">
-        <v>287</v>
+        <v>263</v>
+      </c>
+      <c r="C153" t="s">
+        <v>262</v>
+      </c>
+      <c r="D153" t="s">
+        <v>262</v>
       </c>
       <c r="E153" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -4244,10 +4231,13 @@
         <v>5</v>
       </c>
       <c r="B154" t="s">
-        <v>289</v>
+        <v>265</v>
+      </c>
+      <c r="D154" t="s">
+        <v>264</v>
       </c>
       <c r="E154" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -4255,10 +4245,10 @@
         <v>5</v>
       </c>
       <c r="B155" t="s">
-        <v>291</v>
-      </c>
-      <c r="E155" t="s">
-        <v>290</v>
+        <v>267</v>
+      </c>
+      <c r="C155" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -4266,10 +4256,10 @@
         <v>5</v>
       </c>
       <c r="B156" t="s">
-        <v>293</v>
-      </c>
-      <c r="E156" t="s">
-        <v>292</v>
+        <v>269</v>
+      </c>
+      <c r="C156" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -4277,10 +4267,16 @@
         <v>5</v>
       </c>
       <c r="B157" t="s">
-        <v>295</v>
+        <v>271</v>
+      </c>
+      <c r="C157" t="s">
+        <v>270</v>
+      </c>
+      <c r="D157" t="s">
+        <v>270</v>
       </c>
       <c r="E157" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -4288,10 +4284,16 @@
         <v>5</v>
       </c>
       <c r="B158" t="s">
-        <v>297</v>
+        <v>275</v>
+      </c>
+      <c r="C158" t="s">
+        <v>274</v>
+      </c>
+      <c r="D158" t="s">
+        <v>273</v>
       </c>
       <c r="E158" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -4299,10 +4301,16 @@
         <v>5</v>
       </c>
       <c r="B159" t="s">
-        <v>304</v>
+        <v>278</v>
+      </c>
+      <c r="C159" t="s">
+        <v>277</v>
+      </c>
+      <c r="D159" t="s">
+        <v>277</v>
       </c>
       <c r="E159" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -4310,10 +4318,16 @@
         <v>5</v>
       </c>
       <c r="B160" t="s">
-        <v>305</v>
+        <v>280</v>
+      </c>
+      <c r="C160" t="s">
+        <v>280</v>
+      </c>
+      <c r="D160" t="s">
+        <v>280</v>
       </c>
       <c r="E160" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -4321,10 +4335,16 @@
         <v>5</v>
       </c>
       <c r="B161" t="s">
-        <v>306</v>
+        <v>283</v>
+      </c>
+      <c r="C161" t="s">
+        <v>282</v>
+      </c>
+      <c r="D161" t="s">
+        <v>282</v>
       </c>
       <c r="E161" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -4332,10 +4352,10 @@
         <v>5</v>
       </c>
       <c r="B162" t="s">
-        <v>308</v>
-      </c>
-      <c r="E162" t="s">
-        <v>307</v>
+        <v>285</v>
+      </c>
+      <c r="D162" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
@@ -4343,10 +4363,10 @@
         <v>5</v>
       </c>
       <c r="B163" t="s">
-        <v>314</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>309</v>
+        <v>287</v>
+      </c>
+      <c r="E163" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
@@ -4354,10 +4374,10 @@
         <v>5</v>
       </c>
       <c r="B164" t="s">
-        <v>315</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>310</v>
+        <v>289</v>
+      </c>
+      <c r="E164" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
@@ -4365,10 +4385,10 @@
         <v>5</v>
       </c>
       <c r="B165" t="s">
-        <v>316</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>311</v>
+        <v>291</v>
+      </c>
+      <c r="E165" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
@@ -4376,10 +4396,10 @@
         <v>5</v>
       </c>
       <c r="B166" t="s">
-        <v>317</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>312</v>
+        <v>293</v>
+      </c>
+      <c r="E166" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
@@ -4387,120 +4407,120 @@
         <v>5</v>
       </c>
       <c r="B167" t="s">
-        <v>318</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>313</v>
+        <v>295</v>
+      </c>
+      <c r="E167" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>5</v>
       </c>
-      <c r="B168" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>319</v>
+      <c r="B168" t="s">
+        <v>297</v>
+      </c>
+      <c r="E168" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>5</v>
       </c>
-      <c r="B169" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>320</v>
+      <c r="B169" t="s">
+        <v>304</v>
+      </c>
+      <c r="E169" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>5</v>
       </c>
-      <c r="B170" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>321</v>
+      <c r="B170" t="s">
+        <v>305</v>
+      </c>
+      <c r="E170" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>5</v>
       </c>
-      <c r="B171" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>322</v>
+      <c r="B171" t="s">
+        <v>306</v>
+      </c>
+      <c r="E171" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>5</v>
       </c>
-      <c r="B172" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>323</v>
+      <c r="B172" t="s">
+        <v>308</v>
+      </c>
+      <c r="E172" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>5</v>
       </c>
-      <c r="B173" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>324</v>
+      <c r="B173" t="s">
+        <v>314</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>5</v>
       </c>
-      <c r="B174" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E174" s="3" t="s">
-        <v>325</v>
+      <c r="B174" t="s">
+        <v>315</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>5</v>
       </c>
-      <c r="B175" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>326</v>
+      <c r="B175" t="s">
+        <v>316</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>5</v>
       </c>
-      <c r="B176" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E176" s="3" t="s">
-        <v>327</v>
+      <c r="B176" t="s">
+        <v>317</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>5</v>
       </c>
-      <c r="B177" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>328</v>
+      <c r="B177" t="s">
+        <v>318</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>